<commit_message>
Se edito el nombre de la pestaña. Actualización menor
</commit_message>
<xml_diff>
--- a/Organización/Mejora/Concentrado_Mejoras_2015.xlsx
+++ b/Organización/Mejora/Concentrado_Mejoras_2015.xlsx
@@ -5,14 +5,14 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gus\Desktop\GitHub\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gus\Documents\IWM\CMMI\GitHUB\Organización\Mejora\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="9435" windowHeight="1515"/>
   </bookViews>
   <sheets>
-    <sheet name="Catalogo de cursos" sheetId="7" r:id="rId1"/>
+    <sheet name="Concentrado de cursos" sheetId="7" r:id="rId1"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId2"/>
@@ -213,12 +213,6 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -227,6 +221,12 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -953,8 +953,8 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:AP48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -973,20 +973,20 @@
     <row r="5" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
+      <c r="A8" s="12"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
     </row>
     <row r="9" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
@@ -1011,19 +1011,19 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E11" s="10" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1143,70 +1143,70 @@
       <c r="H28" s="2"/>
     </row>
     <row r="29" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="8"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
+      <c r="A29" s="11"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="8"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
+      <c r="A30" s="11"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="8"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
+      <c r="A31" s="11"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="8"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
+      <c r="A32" s="11"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="8"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
+      <c r="A33" s="11"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="8"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
+      <c r="A34" s="11"/>
+      <c r="B34" s="11"/>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="8"/>
-      <c r="B35" s="8"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
+      <c r="A35" s="11"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>

</xml_diff>

<commit_message>
Se agregó una Mejora
</commit_message>
<xml_diff>
--- a/Organización/Mejora/Concentrado_Mejoras_2015.xlsx
+++ b/Organización/Mejora/Concentrado_Mejoras_2015.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>Nombre</t>
   </si>
@@ -66,6 +66,15 @@
   </si>
   <si>
     <t xml:space="preserve">Aprobado </t>
+  </si>
+  <si>
+    <t>Estimación y Esfuerzo</t>
+  </si>
+  <si>
+    <t>Aclarar como trabajar con la columna de complejidad en la pestaña de Factor de complejidad. Especificando que los valores en esta columna no debían de ser cambiados.</t>
+  </si>
+  <si>
+    <t>Estimaciones y Planeación</t>
   </si>
 </sst>
 </file>
@@ -200,7 +209,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -227,6 +236,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -954,7 +966,7 @@
   <dimension ref="A1:AP48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1027,12 +1039,22 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
+    <row r="12" spans="1:5" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="13" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>

</xml_diff>

<commit_message>
Se agrego una solicitud de mejora
</commit_message>
<xml_diff>
--- a/Organización/Mejora/Concentrado_Mejoras_2015.xlsx
+++ b/Organización/Mejora/Concentrado_Mejoras_2015.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gus\Documents\IWM\CMMI\GitHUB\Organización\Mejora\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9435" windowHeight="1515"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9432" windowHeight="1512"/>
   </bookViews>
   <sheets>
     <sheet name="Concentrado de cursos" sheetId="7" r:id="rId1"/>
@@ -25,12 +20,12 @@
     <definedName name="Modo">[2]Hoja1!$A$1:$A$7</definedName>
     <definedName name="TiposDeActividad">[1]Parametros!$A$2:$A$9</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>Nombre</t>
   </si>
@@ -75,6 +70,17 @@
   </si>
   <si>
     <t>Estimaciones y Planeación</t>
+  </si>
+  <si>
+    <t>Reporte de No conformidades</t>
+  </si>
+  <si>
+    <t>En la plantilla de Reporte de no conformidades 
+1. Quitar la columna de recomendaciones
+2. Agregar todos los procesos de la organización en la lista de la columna de proceso</t>
+  </si>
+  <si>
+    <t>Aseguramiento de la calidad</t>
   </si>
 </sst>
 </file>
@@ -209,7 +215,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -231,13 +237,16 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -718,7 +727,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -753,7 +762,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -965,17 +974,17 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:AP48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12:E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="39.28515625" style="1" customWidth="1"/>
-    <col min="3" max="4" width="19.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" style="1" customWidth="1"/>
-    <col min="6" max="42" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="34" style="1" customWidth="1"/>
+    <col min="2" max="2" width="39.33203125" style="1" customWidth="1"/>
+    <col min="3" max="4" width="19.5546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" style="1" customWidth="1"/>
+    <col min="6" max="42" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -984,28 +993,28 @@
     <row r="4" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+    <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-    </row>
-    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="12"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-    </row>
-    <row r="9" spans="1:5" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+    </row>
+    <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="13"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>0</v>
       </c>
@@ -1022,7 +1031,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>4</v>
       </c>
@@ -1039,11 +1048,11 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="11" t="s">
         <v>13</v>
       </c>
       <c r="C12" s="6" t="s">
@@ -1056,105 +1065,115 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-    </row>
-    <row r="14" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="6"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
     </row>
-    <row r="15" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="6"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
     </row>
-    <row r="16" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="6"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
     </row>
-    <row r="17" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="6"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
     </row>
-    <row r="18" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="6"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
     </row>
-    <row r="19" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="6"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
     </row>
-    <row r="20" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="6"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
     </row>
-    <row r="21" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="6"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
     </row>
-    <row r="22" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="6"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
     </row>
-    <row r="23" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="6"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
     </row>
-    <row r="24" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="6"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
     </row>
-    <row r="25" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="6"/>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
     </row>
-    <row r="26" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="6"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -1164,77 +1183,77 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="11"/>
-      <c r="B29" s="11"/>
-      <c r="C29" s="11"/>
-      <c r="D29" s="11"/>
+    <row r="29" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="12"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="11"/>
-      <c r="B30" s="11"/>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" s="12"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="11"/>
-      <c r="B31" s="11"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="11"/>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" s="12"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="11"/>
-      <c r="B32" s="11"/>
-      <c r="C32" s="11"/>
-      <c r="D32" s="11"/>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" s="12"/>
+      <c r="B32" s="12"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="11"/>
-      <c r="B33" s="11"/>
-      <c r="C33" s="11"/>
-      <c r="D33" s="11"/>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33" s="12"/>
+      <c r="B33" s="12"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="11"/>
-      <c r="B34" s="11"/>
-      <c r="C34" s="11"/>
-      <c r="D34" s="11"/>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34" s="12"/>
+      <c r="B34" s="12"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="11"/>
-      <c r="B35" s="11"/>
-      <c r="C35" s="11"/>
-      <c r="D35" s="11"/>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35" s="12"/>
+      <c r="B35" s="12"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="12"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -1244,7 +1263,7 @@
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -1254,7 +1273,7 @@
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -1264,7 +1283,7 @@
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -1274,7 +1293,7 @@
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -1284,7 +1303,7 @@
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -1294,7 +1313,7 @@
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -1304,7 +1323,7 @@
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -1314,7 +1333,7 @@
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -1324,7 +1343,7 @@
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -1334,7 +1353,7 @@
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -1344,7 +1363,7 @@
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -1354,7 +1373,7 @@
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>

</xml_diff>